<commit_message>
Revised Abstract. Numbers updated
</commit_message>
<xml_diff>
--- a/artefacts/presentation/Presentation_Reference_Tables.xlsx
+++ b/artefacts/presentation/Presentation_Reference_Tables.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Article_Empirical_Study\artefacts\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC30311F-253A-4470-ABB8-7939E3736A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BE371F-9453-4A20-AC28-028C53DC3D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="130" xr2:uid="{0735BFBC-3050-4A4D-9C32-627D721587C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0735BFBC-3050-4A4D-9C32-627D721587C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HP" sheetId="1" r:id="rId1"/>
+    <sheet name="Dell" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="41">
   <si>
     <t xml:space="preserve">Environment </t>
   </si>
@@ -190,7 +191,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -319,9 +320,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -338,14 +339,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -355,24 +353,30 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81424D6-DC54-4F2B-83CF-AE5BCCA82414}">
   <dimension ref="C2:V80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:N56"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,33 +716,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
     </row>
     <row r="3" spans="3:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -1864,25 +1868,25 @@
     </row>
     <row r="27" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="9"/>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="10" t="s">
+      <c r="H27" s="22"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="10" t="s">
+      <c r="K27" s="22"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N27" s="10"/>
+      <c r="N27" s="22"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -1892,160 +1896,160 @@
       <c r="V27" s="1"/>
     </row>
     <row r="28" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="12"/>
-      <c r="D28" s="13" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="13" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="13" t="s">
+      <c r="I28" s="10"/>
+      <c r="J28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="13" t="s">
+      <c r="L28" s="10"/>
+      <c r="M28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <v>0.44800000000000001</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="14">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="15">
+      <c r="F29" s="15"/>
+      <c r="G29" s="14">
         <v>0.47799999999999998</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="15">
+      <c r="I29" s="15"/>
+      <c r="J29" s="14">
         <v>0.443</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="14">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="L29" s="16"/>
-      <c r="M29" s="15">
+      <c r="L29" s="15"/>
+      <c r="M29" s="14">
         <v>0.439</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N29" s="14">
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="30" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="17">
         <v>0.41499999999999998</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="17">
         <v>0.19600000000000001</v>
       </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="18">
+      <c r="F30" s="18"/>
+      <c r="G30" s="17">
         <v>0.46200000000000002</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="17">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I30" s="19"/>
-      <c r="J30" s="18">
+      <c r="I30" s="18"/>
+      <c r="J30" s="17">
         <v>0.34300000000000003</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="17">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="L30" s="19"/>
-      <c r="M30" s="18">
+      <c r="L30" s="18"/>
+      <c r="M30" s="17">
         <v>0.32500000000000001</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N30" s="17">
         <v>6.3E-2</v>
       </c>
     </row>
     <row r="31" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="17">
         <v>0.44700000000000001</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="17">
         <v>0.14699999999999999</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="18">
+      <c r="F31" s="18"/>
+      <c r="G31" s="17">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="17">
         <v>0.09</v>
       </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="18">
+      <c r="I31" s="18"/>
+      <c r="J31" s="17">
         <v>0.33400000000000002</v>
       </c>
-      <c r="K31" s="18">
+      <c r="K31" s="17">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="18">
+      <c r="L31" s="18"/>
+      <c r="M31" s="17">
         <v>0.375</v>
       </c>
-      <c r="N31" s="18">
+      <c r="N31" s="17">
         <v>0.107</v>
       </c>
     </row>
     <row r="32" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="20">
         <v>0.86599999999999999</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="20">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="21">
+      <c r="F32" s="21"/>
+      <c r="G32" s="20">
         <v>0.84699999999999998</v>
       </c>
-      <c r="H32" s="21">
+      <c r="H32" s="20">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="21">
+      <c r="I32" s="21"/>
+      <c r="J32" s="20">
         <v>0.84199999999999997</v>
       </c>
-      <c r="K32" s="21">
+      <c r="K32" s="20">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="L32" s="22"/>
-      <c r="M32" s="21">
+      <c r="L32" s="21"/>
+      <c r="M32" s="20">
         <v>0.85199999999999998</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="20">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -2064,205 +2068,205 @@
     </row>
     <row r="35" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="9"/>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="10" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="10" t="s">
+      <c r="H35" s="22"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="10" t="s">
+      <c r="K35" s="22"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N35" s="10"/>
+      <c r="N35" s="22"/>
     </row>
     <row r="36" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="12"/>
-      <c r="D36" s="13" t="s">
+      <c r="C36" s="11"/>
+      <c r="D36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="13" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="13" t="s">
+      <c r="I36" s="10"/>
+      <c r="J36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="13" t="s">
+      <c r="L36" s="10"/>
+      <c r="M36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N36" s="13" t="s">
+      <c r="N36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="14">
         <v>0.40500000000000003</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="14">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F37" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37" s="15">
+      <c r="F37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="14">
         <v>0.372</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I37" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="15">
+      <c r="I37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="14">
         <v>0.379</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="14">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="L37" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M37" s="15">
+      <c r="L37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M37" s="14">
         <v>0.39100000000000001</v>
       </c>
-      <c r="N37" s="15">
+      <c r="N37" s="14">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="17">
         <v>0.34799999999999998</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="17">
         <v>0.217</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="18">
+      <c r="F38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="17">
         <v>0.35599999999999998</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="17">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I38" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J38" s="18">
+      <c r="I38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="17">
         <v>0.26</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="17">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="L38" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M38" s="18">
+      <c r="L38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M38" s="17">
         <v>0.248</v>
       </c>
-      <c r="N38" s="18">
+      <c r="N38" s="17">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="39" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="17">
         <v>0.38500000000000001</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="17">
         <v>0.17499999999999999</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="18">
+      <c r="F39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="17">
         <v>0.19600000000000001</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="17">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J39" s="18">
+      <c r="I39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="17">
         <v>0.23499999999999999</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="17">
         <v>0.08</v>
       </c>
-      <c r="L39" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M39" s="18">
+      <c r="L39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="17">
         <v>0.28899999999999998</v>
       </c>
-      <c r="N39" s="18">
+      <c r="N39" s="17">
         <v>0.11</v>
       </c>
     </row>
     <row r="40" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="20">
         <v>0.94399999999999995</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="20">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F40" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="21">
+      <c r="F40" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="20">
         <v>0.85799999999999998</v>
       </c>
-      <c r="H40" s="21">
+      <c r="H40" s="20">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I40" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="21">
+      <c r="I40" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="20">
         <v>0.88600000000000001</v>
       </c>
-      <c r="K40" s="21">
+      <c r="K40" s="20">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="L40" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="M40" s="21">
+      <c r="L40" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M40" s="20">
         <v>0.91600000000000004</v>
       </c>
-      <c r="N40" s="21">
+      <c r="N40" s="20">
         <v>0.03</v>
       </c>
     </row>
@@ -2281,205 +2285,205 @@
     </row>
     <row r="43" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="9"/>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="10" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="10" t="s">
+      <c r="H43" s="22"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K43" s="10"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="10" t="s">
+      <c r="K43" s="22"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N43" s="10"/>
+      <c r="N43" s="22"/>
     </row>
     <row r="44" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="12"/>
-      <c r="D44" s="13" t="s">
+      <c r="C44" s="11"/>
+      <c r="D44" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="13" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="13" t="s">
+      <c r="I44" s="10"/>
+      <c r="J44" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="13" t="s">
+      <c r="K44" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L44" s="11"/>
-      <c r="M44" s="13" t="s">
+      <c r="L44" s="10"/>
+      <c r="M44" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N44" s="13" t="s">
+      <c r="N44" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="14">
         <v>0.45100000000000001</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="14">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="F45" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="15">
+      <c r="F45" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="14">
         <v>0.52400000000000002</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="14">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="I45" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J45" s="15">
+      <c r="I45" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J45" s="14">
         <v>0.47199999999999998</v>
       </c>
-      <c r="K45" s="15">
+      <c r="K45" s="14">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="L45" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M45" s="15">
+      <c r="L45" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M45" s="14">
         <v>0.45600000000000002</v>
       </c>
-      <c r="N45" s="15">
+      <c r="N45" s="14">
         <v>6.3E-2</v>
       </c>
     </row>
     <row r="46" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="17">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="17">
         <v>0.17199999999999999</v>
       </c>
-      <c r="F46" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="18">
+      <c r="F46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="17">
         <v>0.53</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="17">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I46" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J46" s="18">
+      <c r="I46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J46" s="17">
         <v>0.38900000000000001</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="17">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="L46" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M46" s="18">
+      <c r="L46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" s="17">
         <v>0.35699999999999998</v>
       </c>
-      <c r="N46" s="18">
+      <c r="N46" s="17">
         <v>5.5E-2</v>
       </c>
     </row>
     <row r="47" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="17">
         <v>0.45</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="17">
         <v>0.14599999999999999</v>
       </c>
-      <c r="F47" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="18">
+      <c r="F47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="17">
         <v>0.32700000000000001</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="17">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="I47" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J47" s="18">
+      <c r="I47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="17">
         <v>0.34899999999999998</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="17">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="L47" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M47" s="18">
+      <c r="L47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M47" s="17">
         <v>0.38400000000000001</v>
       </c>
-      <c r="N47" s="18">
+      <c r="N47" s="17">
         <v>0.106</v>
       </c>
     </row>
     <row r="48" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="20">
         <v>0.84199999999999997</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E48" s="20">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="F48" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="21">
+      <c r="F48" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="20">
         <v>0.88</v>
       </c>
-      <c r="H48" s="21">
+      <c r="H48" s="20">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="I48" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J48" s="21">
+      <c r="I48" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48" s="20">
         <v>0.84799999999999998</v>
       </c>
-      <c r="K48" s="21">
+      <c r="K48" s="20">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="L48" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="M48" s="21">
+      <c r="L48" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M48" s="20">
         <v>0.84099999999999997</v>
       </c>
-      <c r="N48" s="21">
+      <c r="N48" s="20">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -2494,205 +2498,205 @@
     </row>
     <row r="51" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="9"/>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="10"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="10" t="s">
+      <c r="E51" s="22"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="10" t="s">
+      <c r="H51" s="22"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K51" s="10"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="10" t="s">
+      <c r="K51" s="22"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N51" s="10"/>
+      <c r="N51" s="22"/>
     </row>
     <row r="52" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="12"/>
-      <c r="D52" s="13" t="s">
+      <c r="C52" s="11"/>
+      <c r="D52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="13" t="s">
+      <c r="F52" s="10"/>
+      <c r="G52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="H52" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I52" s="11"/>
-      <c r="J52" s="13" t="s">
+      <c r="I52" s="10"/>
+      <c r="J52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="13" t="s">
+      <c r="K52" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L52" s="11"/>
-      <c r="M52" s="13" t="s">
+      <c r="L52" s="10"/>
+      <c r="M52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N52" s="13" t="s">
+      <c r="N52" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="15">
+      <c r="D53" s="14">
         <v>0.48299999999999998</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="14">
         <v>0.10100000000000001</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G53" s="15">
+      <c r="F53" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="14">
         <v>0.44700000000000001</v>
       </c>
-      <c r="H53" s="15">
+      <c r="H53" s="14">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I53" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J53" s="15">
+      <c r="I53" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J53" s="14">
         <v>0.41899999999999998</v>
       </c>
-      <c r="K53" s="15">
+      <c r="K53" s="14">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L53" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M53" s="15">
+      <c r="L53" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M53" s="14">
         <v>0.435</v>
       </c>
-      <c r="N53" s="15">
+      <c r="N53" s="14">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="54" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="18">
+      <c r="D54" s="17">
         <v>0.47399999999999998</v>
       </c>
-      <c r="E54" s="18">
+      <c r="E54" s="17">
         <v>0.248</v>
       </c>
-      <c r="F54" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G54" s="18">
+      <c r="F54" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="17">
         <v>0.36499999999999999</v>
       </c>
-      <c r="H54" s="18">
+      <c r="H54" s="17">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="I54" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J54" s="18">
+      <c r="I54" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="17">
         <v>0.28899999999999998</v>
       </c>
-      <c r="K54" s="18">
+      <c r="K54" s="17">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="L54" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M54" s="18">
+      <c r="L54" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M54" s="17">
         <v>0.30599999999999999</v>
       </c>
-      <c r="N54" s="18">
+      <c r="N54" s="17">
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="55" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="18">
+      <c r="D55" s="17">
         <v>0.498</v>
       </c>
-      <c r="E55" s="18">
+      <c r="E55" s="17">
         <v>0.121</v>
       </c>
-      <c r="F55" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" s="18">
+      <c r="F55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="17">
         <v>0.35399999999999998</v>
       </c>
-      <c r="H55" s="18">
+      <c r="H55" s="17">
         <v>0.10299999999999999</v>
       </c>
-      <c r="I55" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J55" s="18">
+      <c r="I55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="17">
         <v>0.39</v>
       </c>
-      <c r="K55" s="18">
+      <c r="K55" s="17">
         <v>0.10100000000000001</v>
       </c>
-      <c r="L55" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M55" s="18">
+      <c r="L55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M55" s="17">
         <v>0.436</v>
       </c>
-      <c r="N55" s="18">
+      <c r="N55" s="17">
         <v>0.104</v>
       </c>
     </row>
     <row r="56" spans="3:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="20">
         <v>0.85899999999999999</v>
       </c>
-      <c r="E56" s="21">
+      <c r="E56" s="20">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F56" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G56" s="21">
+      <c r="F56" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="20">
         <v>0.73899999999999999</v>
       </c>
-      <c r="H56" s="21">
+      <c r="H56" s="20">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I56" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J56" s="21">
+      <c r="I56" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="20">
         <v>0.78100000000000003</v>
       </c>
-      <c r="K56" s="21">
+      <c r="K56" s="20">
         <v>5.5E-2</v>
       </c>
-      <c r="L56" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="M56" s="21">
+      <c r="L56" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M56" s="20">
         <v>0.82199999999999995</v>
       </c>
-      <c r="N56" s="21">
+      <c r="N56" s="20">
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
@@ -2722,6 +2726,14 @@
     <row r="80" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="G51:H51"/>
     <mergeCell ref="J51:K51"/>
@@ -2734,14 +2746,6 @@
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="M43:N43"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="M27:N27"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:V5">
     <cfRule type="colorScale" priority="21">
@@ -2959,7 +2963,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F50 I50 L50">
+  <conditionalFormatting sqref="I50 F50 L50">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2985,4 +2989,1580 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D258FC61-8A48-454B-8812-FDF55D5DC3CA}">
+  <dimension ref="C2:V46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" customWidth="1"/>
+    <col min="9" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" customWidth="1"/>
+    <col min="19" max="22" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+    </row>
+    <row r="3" spans="3:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.65999999999999903</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.79458237840590695</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.90603500171998597</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>0.37084249084248999</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.238827920070313</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.30137205201059603</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="P5" s="1">
+        <v>3.8095238095238002E-2</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1">
+        <v>0.25749999999999901</v>
+      </c>
+      <c r="T5" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0.100882117882117</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.15419164169164101</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.95709956709956701</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.97047887072277295</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.96232015669515603</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
+        <v>0.52339147901723604</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.49500524283823499</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.51079730481189201</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <v>0.433193277310924</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.745</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.54781144781144697</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.47275641025641002</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="U6" s="1">
+        <v>6.47759197324414E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0.103977272727272</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.86869000564652699</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.92291081956425103</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.88953666863149605</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
+        <v>0.33715728715728699</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.105</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.15360253802967899</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.21965187590187499</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>9.5446640316205505E-2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.17232142857142799</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="U7" s="1">
+        <v>9.1017677974199601E-2</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.13439685314685301</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.91721626199886996</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.95189665883369801</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.93071021571021495</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>0.465809966177613</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.45535239869949901</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.46100688439398102</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1">
+        <v>0.50519568151147098</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.66894603545684705</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.56002613342729601</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1">
+        <v>0.57443548759910301</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.58151167044836105</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.57657542204276602</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.96152261781905701</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.90673420383946701</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.93849120082815696</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1">
+        <v>0.50540358171937105</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.66791555159084104</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.55988351119165003</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1">
+        <v>0.57225534191209204</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0.60556172509660799</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.58452025385215001</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.89190661436199103</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.91386217645718504</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.90025183150183097</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <v>0.437615119658463</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.45499999999999902</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.44396958166841499</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.43962835870511002</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1">
+        <v>0.50006747638326499</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.66216637443989801</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.554344315245478</v>
+      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1">
+        <v>0.50872249589490903</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.59528799771656904</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.53999960782415102</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.75634155297198702</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.84531003731786802</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.78944656219753495</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>0.47123918865791897</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.45880658388360501</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.46577175441305801</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>0.501212751212751</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.66313841295231002</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.55545802711500303</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1">
+        <v>0.45482683982683902</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.24878745343150199</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.337830051892551</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.830533090098307</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.994999999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.90489336525736896</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.858673805698277</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1">
+        <v>0.49809163059162997</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.51268967874230997</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.50363962249644401</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1">
+        <v>0.49345479082321098</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.65178258328462801</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.54655567300916097</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1">
+        <v>0.53846461509504895</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0.58904341484553002</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.55725419911320895</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.77088274044795702</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.80999999999999905</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.78952272911433397</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.77813644688644601</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
+        <v>0.54811393793087104</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.56006682327676605</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.55181521360956798</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="P14" s="1">
+        <v>3.7229437229437203E-2</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>7.73809523809523E-2</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1">
+        <v>0.53857531357531296</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.38246733517172798</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.46120459401709402</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.75661980334655798</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.88545697884416896</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
+        <v>0.58015665862671295</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.61629354891531396</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.59343543133065102</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O15" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>6.2121212121212098E-2</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.11706349206349199</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1">
+        <v>0.55560367607968197</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.51037142013372905</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.53515845567475995</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.946370214752567</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.85086829421194698</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.90529033799914804</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
+        <v>0.454349861225954</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.43661312329790097</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.446409297224514</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="O16" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P16" s="1">
+        <v>4.2424242424242399E-2</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>7.3412698412698402E-2</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1">
+        <v>0.38583333333333297</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="U16" s="1">
+        <v>9.8829851308112102E-2</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.16768543956043899</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.72537055281882801</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.821926180474151</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.76102025218900304</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
+        <v>0.51760881146716997</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.505</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.51013484537874698</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.51430180930180902</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1">
+        <v>0.96934001670843695</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0.91878808797935796</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.94820442238920499</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1">
+        <v>0.33999999999999903</v>
+      </c>
+      <c r="T17" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.112045621045621</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.179872904872904</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.80500606754039195</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.869999999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.83504921435154</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.81649311257069801</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1">
+        <v>0.79166666666666596</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0.20701581027667901</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.36830357142857101</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1">
+        <v>0.50380952380952304</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0.16999999999999901</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0.24968659565211199</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0.35305666555666498</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.74829401669134399</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.72182188496753896</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.73708815640880798</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1">
+        <v>0.49615566983988002</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.65182154685369098</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.54855343300110704</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1">
+        <v>0.489610460663092</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.64020417789066397</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.54045327781501895</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1">
+        <v>0.51629857071033503</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0.40102365442922699</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.46047066818704901</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.81935319582378396</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.91867690058479501</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1">
+        <v>0.50399299530878405</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.65341743251445095</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.55470439703990404</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>2.8138528138528102E-2</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>5.95238095238095E-2</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1">
+        <v>0.49158008658008601</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0.27991777143056301</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0.37324637168387098</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="3:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+    </row>
+    <row r="32" spans="3:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+    </row>
+    <row r="33" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+    </row>
+    <row r="34" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+    </row>
+    <row r="35" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+    </row>
+    <row r="36" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+    </row>
+    <row r="37" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+    </row>
+    <row r="38" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+    </row>
+    <row r="39" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+    </row>
+    <row r="40" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+    </row>
+    <row r="41" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+    </row>
+    <row r="42" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+    </row>
+    <row r="43" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+    </row>
+    <row r="44" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+    </row>
+    <row r="45" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+    </row>
+    <row r="46" spans="4:22" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="S2:V2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5:V5">
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:V6">
+    <cfRule type="colorScale" priority="126">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:V8">
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:V9">
+    <cfRule type="colorScale" priority="130">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:V10">
+    <cfRule type="colorScale" priority="132">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:V11">
+    <cfRule type="colorScale" priority="134">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:V12">
+    <cfRule type="colorScale" priority="136">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:V13">
+    <cfRule type="colorScale" priority="138">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:V14">
+    <cfRule type="colorScale" priority="140">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:V15">
+    <cfRule type="colorScale" priority="142">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:V16">
+    <cfRule type="colorScale" priority="144">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:V18">
+    <cfRule type="colorScale" priority="146">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:V19">
+    <cfRule type="colorScale" priority="148">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:V20">
+    <cfRule type="colorScale" priority="150">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:V21">
+    <cfRule type="colorScale" priority="152">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:V23">
+    <cfRule type="colorScale" priority="154">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>